<commit_message>
finished chapter 6 woohoo yipee
</commit_message>
<xml_diff>
--- a/starwars_Ch6_max.xlsx
+++ b/starwars_Ch6_max.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BolognaColonel\workspace\excel\data\starwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF22CB2-4D6F-4CC2-AF6E-753452D7CB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EF82CF-5521-441D-9DF8-8E16F3B94559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19230" yWindow="75" windowWidth="19095" windowHeight="20850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="301">
   <si>
     <t>name</t>
   </si>
@@ -942,6 +942,27 @@
   </si>
   <si>
     <t>With the functions</t>
+  </si>
+  <si>
+    <t>height_freq</t>
+  </si>
+  <si>
+    <t>diff_mean</t>
+  </si>
+  <si>
+    <t>diff_mean_sqd</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Std Deviation</t>
+  </si>
+  <si>
+    <t>90th Percentile</t>
+  </si>
+  <si>
+    <t>1st Quartile</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1010,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,6 +1029,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1021,7 +1048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1032,6 +1059,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,7 +1408,7 @@
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K33" ca="1" si="2">IFERROR(TODAY()-$J2, "NA")</f>
-        <v>39102</v>
+        <v>39103</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>14</v>
@@ -1456,7 +1484,7 @@
       </c>
       <c r="K3" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>5157</v>
+        <v>5158</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>21</v>
@@ -1532,7 +1560,7 @@
       </c>
       <c r="K4" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>33992</v>
+        <v>33993</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>21</v>
@@ -1608,7 +1636,7 @@
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>30743.499999999967</v>
+        <v>30744.499999999967</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>32</v>
@@ -1684,7 +1712,7 @@
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>39102</v>
+        <v>39103</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>36</v>
@@ -1760,7 +1788,7 @@
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>27057</v>
+        <v>27058</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>41</v>
@@ -1836,7 +1864,7 @@
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>28882</v>
+        <v>28883</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>36</v>
@@ -1988,7 +2016,7 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>37277</v>
+        <v>37278</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>48</v>
@@ -2064,7 +2092,7 @@
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>25232</v>
+        <v>25233</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>50</v>
@@ -2140,7 +2168,7 @@
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>30743.499999999967</v>
+        <v>30744.499999999967</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>14</v>
@@ -2216,7 +2244,7 @@
       </c>
       <c r="K13" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>22677</v>
+        <v>22678</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>56</v>
@@ -2292,7 +2320,7 @@
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-26963</v>
+        <v>-26962</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>36</v>
@@ -2368,7 +2396,7 @@
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>35452</v>
+        <v>35453</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>36</v>
@@ -2444,7 +2472,7 @@
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>29977</v>
+        <v>29978</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>21</v>
@@ -2520,7 +2548,7 @@
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-172963</v>
+        <v>-172962</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>21</v>
@@ -2596,7 +2624,7 @@
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>38372</v>
+        <v>38373</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>36</v>
@@ -2748,7 +2776,7 @@
       </c>
       <c r="K20" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-281003</v>
+        <v>-281002</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>33</v>
@@ -2824,7 +2852,7 @@
       </c>
       <c r="K21" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>16107</v>
+        <v>16108</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>85</v>
@@ -2900,7 +2928,7 @@
       </c>
       <c r="K22" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>34539.5</v>
+        <v>34540.5</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>48</v>
@@ -2976,7 +3004,7 @@
       </c>
       <c r="K23" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>40562</v>
+        <v>40563</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>32</v>
@@ -3052,7 +3080,7 @@
       </c>
       <c r="K24" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>26692</v>
+        <v>26693</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>32</v>
@@ -3128,7 +3156,7 @@
       </c>
       <c r="K25" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>34722</v>
+        <v>34723</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>48</v>
@@ -3204,7 +3232,7 @@
       </c>
       <c r="K26" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>32532</v>
+        <v>32533</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>32</v>
@@ -3280,7 +3308,7 @@
       </c>
       <c r="K27" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>31072</v>
+        <v>31073</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>32</v>
@@ -3356,7 +3384,7 @@
       </c>
       <c r="K28" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>28517</v>
+        <v>28518</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>109</v>
@@ -3508,7 +3536,7 @@
       </c>
       <c r="K30" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>43117</v>
+        <v>43118</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>36</v>
@@ -3660,7 +3688,7 @@
       </c>
       <c r="K32" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>12457</v>
+        <v>12458</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>36</v>
@@ -3812,7 +3840,7 @@
       </c>
       <c r="K34" s="5">
         <f t="shared" ref="K34:K65" ca="1" si="12">IFERROR(TODAY()-$J34, "NA")</f>
-        <v>12822</v>
+        <v>12823</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>14</v>
@@ -3888,7 +3916,7 @@
       </c>
       <c r="K35" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>27057</v>
+        <v>27058</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>32</v>
@@ -4344,7 +4372,7 @@
       </c>
       <c r="K41" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>23407</v>
+        <v>23408</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>48</v>
@@ -4420,7 +4448,7 @@
       </c>
       <c r="K42" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>19757</v>
+        <v>19758</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>48</v>
@@ -4496,7 +4524,7 @@
       </c>
       <c r="K43" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>26327</v>
+        <v>26328</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>32</v>
@@ -4648,7 +4676,7 @@
       </c>
       <c r="K45" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>28517</v>
+        <v>28518</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>32</v>
@@ -4952,7 +4980,7 @@
       </c>
       <c r="K49" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>19757</v>
+        <v>19758</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>32</v>
@@ -5028,7 +5056,7 @@
       </c>
       <c r="K50" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>12457</v>
+        <v>12458</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>33</v>
@@ -5484,7 +5512,7 @@
       </c>
       <c r="K56" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>38007</v>
+        <v>38008</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>32</v>
@@ -5788,7 +5816,7 @@
       </c>
       <c r="K60" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>16107</v>
+        <v>16108</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>36</v>
@@ -5940,7 +5968,7 @@
       </c>
       <c r="K62" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>24867</v>
+        <v>24868</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>48</v>
@@ -6016,7 +6044,7 @@
       </c>
       <c r="K63" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>31437</v>
+        <v>31438</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>48</v>
@@ -6168,7 +6196,7 @@
       </c>
       <c r="K65" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>8807</v>
+        <v>8808</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>33</v>
@@ -6244,7 +6272,7 @@
       </c>
       <c r="K66" s="5">
         <f t="shared" ref="K66:K88" ca="1" si="15">IFERROR(TODAY()-$J66, "NA")</f>
-        <v>21582</v>
+        <v>21583</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>48</v>
@@ -6320,7 +6348,7 @@
       </c>
       <c r="K67" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>21947</v>
+        <v>21948</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>48</v>
@@ -7916,7 +7944,7 @@
       </c>
       <c r="K88" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>29247</v>
+        <v>29248</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>36</v>
@@ -7974,7 +8002,7 @@
       </c>
       <c r="C92">
         <f ca="1">DATEDIF($B92, TODAY(), "D")</f>
-        <v>9738</v>
+        <v>9739</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -7988,7 +8016,7 @@
       </c>
       <c r="C93">
         <f t="shared" ref="C93:C98" ca="1" si="23">DATEDIF($B93, TODAY(), "D")</f>
-        <v>8645</v>
+        <v>8646</v>
       </c>
     </row>
     <row r="94" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8000,7 +8028,7 @@
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="23"/>
-        <v>7546</v>
+        <v>7547</v>
       </c>
     </row>
     <row r="95" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8012,7 +8040,7 @@
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="23"/>
-        <v>17767</v>
+        <v>17768</v>
       </c>
     </row>
     <row r="96" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8024,7 +8052,7 @@
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="23"/>
-        <v>16675</v>
+        <v>16676</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8036,7 +8064,7 @@
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="23"/>
-        <v>15576</v>
+        <v>15577</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8048,7 +8076,7 @@
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="23"/>
-        <v>3681</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8958,22 +8986,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2BC748-F643-4C71-8674-6F8571EF4D1F}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>288</v>
       </c>
@@ -8981,10 +9011,19 @@
         <v>287</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8994,8 +9033,20 @@
       <c r="C2">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>COUNTIF($C$2:$C$82, C2)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>$H$10-C2</f>
+        <v>108.35802469135803</v>
+      </c>
+      <c r="F2">
+        <f>E2^2</f>
+        <v>11741.461515012956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9005,13 +9056,25 @@
       <c r="C3">
         <v>79</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">COUNTIF($C$2:$C$82, C3)</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>$H$10-C3</f>
+        <v>95.358024691358025</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">E3^2</f>
+        <v>9093.1528730376467</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9021,17 +9084,29 @@
       <c r="C4">
         <v>88</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>$H$10-C4</f>
+        <v>86.358024691358025</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>7457.7084285932024</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9041,16 +9116,32 @@
       <c r="C5">
         <v>94</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>$H$10-C5</f>
+        <v>80.358024691358025</v>
+      </c>
       <c r="F5">
+        <f t="shared" si="1"/>
+        <v>6457.4121322969058</v>
+      </c>
+      <c r="H5">
         <f>SUM(C2:C82)/COUNT(C2:C82)</f>
         <v>174.35802469135803</v>
       </c>
-      <c r="G5" cm="1">
-        <f t="array" ref="G5">VLOOKUP(IF(ISODD(COUNT(A2:A82)),CEILING(COUNT(A2:A82)/2,1), COUNT(A2:A82/2,1)),A2:C82,3,FALSE)</f>
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">VLOOKUP(IF(ISODD(COUNT(A2:A82)),CEILING(COUNT(A2:A82)/2,1), COUNT(A2:A82/2,1)),A2:C82,3,FALSE)</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>_xlfn.XLOOKUP(MAX(D2:D82),D2:D82,C2:C82,"Not Found")</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9060,9 +9151,20 @@
       <c r="C6">
         <v>96</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f>$H$10-C6</f>
+        <v>78.358024691358025</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>6139.980033531474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9072,8 +9174,20 @@
       <c r="C7">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f>$H$10-C7</f>
+        <v>78.358024691358025</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6139.980033531474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9083,9 +9197,25 @@
       <c r="C8">
         <v>97</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>$H$10-C8</f>
+        <v>77.358024691358025</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>5984.263984148758</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9095,13 +9225,29 @@
       <c r="C9">
         <v>112</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>$H$10-C9</f>
+        <v>62.358024691358025</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3888.5232434080172</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9111,17 +9257,32 @@
       <c r="C10">
         <v>122</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>$H$10-C10</f>
+        <v>52.358024691358025</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2741.3627495808569</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(C2:C82)</f>
+        <v>174.35802469135803</v>
+      </c>
+      <c r="I10" s="1">
+        <f>MEDIAN(C2:C82)</f>
+        <v>180</v>
+      </c>
+      <c r="J10" cm="1">
+        <f t="array" ref="J10">_xlfn.MODE.MULT(C2:C82)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9131,8 +9292,20 @@
       <c r="C11">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>$H$10-C11</f>
+        <v>37.358024691358025</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1395.622008840116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9142,8 +9315,20 @@
       <c r="C12">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>$H$10-C12</f>
+        <v>24.358024691358025</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>593.31336686480722</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9153,8 +9338,20 @@
       <c r="C13">
         <v>150</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>$H$10-C13</f>
+        <v>24.358024691358025</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>593.31336686480722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9164,8 +9361,20 @@
       <c r="C14">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f>$H$10-C14</f>
+        <v>17.358024691358025</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>301.30102118579487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9175,8 +9384,20 @@
       <c r="C15">
         <v>160</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f>$H$10-C15</f>
+        <v>14.358024691358025</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>206.15287303764671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9186,8 +9407,25 @@
       <c r="C16">
         <v>163</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f>$H$10-C16</f>
+        <v>11.358024691358025</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>129.00472488949856</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9197,9 +9435,23 @@
       <c r="C17">
         <v>163</v>
       </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f>$H$10-C17</f>
+        <v>11.358024691358025</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>129.00472488949856</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9209,8 +9461,24 @@
       <c r="C18">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f>$H$10-C18</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>87.57262612406646</v>
+      </c>
+      <c r="H18">
+        <f>AVERAGE(F2:F82)</f>
+        <v>1194.0570035055634</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9220,8 +9488,21 @@
       <c r="C19">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <f>$H$10-C19</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>87.57262612406646</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9231,8 +9512,20 @@
       <c r="C20">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f>$H$10-C20</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>87.57262612406646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9242,8 +9535,25 @@
       <c r="C21">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f>$H$10-C21</f>
+        <v>8.3580246913580254</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>69.856576741350409</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9253,8 +9563,26 @@
       <c r="C22">
         <v>167</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f>$H$10-C22</f>
+        <v>7.3580246913580254</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>54.140527358634365</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9264,8 +9592,28 @@
       <c r="C23">
         <v>167</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f>$H$10-C23</f>
+        <v>7.3580246913580254</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>54.140527358634365</v>
+      </c>
+      <c r="H23">
+        <f>_xlfn.VAR.P(E2:E82)</f>
+        <v>1194.0570035055632</v>
+      </c>
+      <c r="I23">
+        <f>_xlfn.STDEV.P(C2:C82)</f>
+        <v>34.555129915912097</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9275,8 +9623,24 @@
       <c r="C24">
         <v>168</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f>$H$10-C24</f>
+        <v>6.3580246913580254</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>40.424477975918315</v>
+      </c>
+      <c r="H24" t="str">
+        <f>"sqrt: "&amp;SQRT(H23)</f>
+        <v>sqrt: 34.5551299159121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9286,8 +9650,20 @@
       <c r="C25">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f>$H$10-C25</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9297,8 +9673,20 @@
       <c r="C26">
         <v>170</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f>$H$10-C26</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9308,8 +9696,20 @@
       <c r="C27">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <f>$H$10-C27</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9319,8 +9719,20 @@
       <c r="C28">
         <v>170</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <f>$H$10-C28</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9330,8 +9742,20 @@
       <c r="C29">
         <v>171</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f>$H$10-C29</f>
+        <v>3.3580246913580254</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>11.276329827770162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9341,8 +9765,25 @@
       <c r="C30">
         <v>172</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f>$H$10-C30</f>
+        <v>2.3580246913580254</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>5.5602804450541106</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9352,8 +9793,26 @@
       <c r="C31">
         <v>173</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f>$H$10-C31</f>
+        <v>1.3580246913580254</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>1.8442310623380602</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9363,8 +9822,28 @@
       <c r="C32">
         <v>175</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f>$H$10-C32</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.41213229690595854</v>
+      </c>
+      <c r="H32">
+        <f>VLOOKUP(CEILING(COUNT(C2:C82)*0.9,1),A2:F82,3,TRUE)</f>
+        <v>206</v>
+      </c>
+      <c r="I32">
+        <f>VLOOKUP(CEILING(COUNT(C2:C82)*0.25,1),A2:F82,3,TRUE)</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9374,8 +9853,20 @@
       <c r="C33">
         <v>175</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f>$H$10-C33</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.41213229690595854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9385,8 +9876,20 @@
       <c r="C34">
         <v>175</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <f>$H$10-C34</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.41213229690595854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9396,8 +9899,25 @@
       <c r="C35">
         <v>177</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f>$H$10-C35</f>
+        <v>-2.6419753086419746</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>6.9800335314738566</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9407,8 +9927,26 @@
       <c r="C36">
         <v>178</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <f>$H$10-C36</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>13.263984148757807</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9418,8 +9956,28 @@
       <c r="C37">
         <v>178</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <f>$H$10-C37</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>13.263984148757807</v>
+      </c>
+      <c r="H37">
+        <f>_xlfn.PERCENTILE.INC(C2:C82,0.9)</f>
+        <v>206</v>
+      </c>
+      <c r="I37">
+        <f>_xlfn.PERCENTILE.INC(C2:C82,0.25)</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9429,8 +9987,20 @@
       <c r="C38">
         <v>178</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <f>$H$10-C38</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9440,8 +10010,20 @@
       <c r="C39">
         <v>178</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <f>$H$10-C39</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9451,8 +10033,20 @@
       <c r="C40">
         <v>180</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <f>$H$10-C40</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9462,8 +10056,20 @@
       <c r="C41">
         <v>180</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <f>$H$10-C41</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9473,8 +10079,20 @@
       <c r="C42">
         <v>180</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <f>$H$10-C42</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -9484,8 +10102,20 @@
       <c r="C43">
         <v>180</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <f>$H$10-C43</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -9495,8 +10125,20 @@
       <c r="C44">
         <v>180</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <f>$H$10-C44</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -9506,8 +10148,20 @@
       <c r="C45">
         <v>182</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f>$H$10-C45</f>
+        <v>-7.6419753086419746</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>58.399786617893604</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -9517,8 +10171,20 @@
       <c r="C46">
         <v>183</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <f>$H$10-C46</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -9528,8 +10194,20 @@
       <c r="C47">
         <v>183</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E47">
+        <f>$H$10-C47</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -9539,8 +10217,20 @@
       <c r="C48">
         <v>183</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <f>$H$10-C48</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -9550,8 +10240,20 @@
       <c r="C49">
         <v>183</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <f>$H$10-C49</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -9561,8 +10263,20 @@
       <c r="C50">
         <v>183</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <f>$H$10-C50</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -9572,8 +10286,20 @@
       <c r="C51">
         <v>183</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <f>$H$10-C51</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -9583,8 +10309,20 @@
       <c r="C52">
         <v>183</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E52">
+        <f>$H$10-C52</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -9594,8 +10332,20 @@
       <c r="C53">
         <v>184</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <f>$H$10-C53</f>
+        <v>-9.6419753086419746</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>92.967687852461495</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -9605,8 +10355,20 @@
       <c r="C54">
         <v>185</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <f>$H$10-C54</f>
+        <v>-10.641975308641975</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>113.25163846974544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9616,8 +10378,20 @@
       <c r="C55">
         <v>188</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <f>$H$10-C55</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9627,8 +10401,20 @@
       <c r="C56">
         <v>188</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <f>$H$10-C56</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9638,8 +10424,20 @@
       <c r="C57">
         <v>188</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <f>$H$10-C57</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9649,8 +10447,20 @@
       <c r="C58">
         <v>188</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E58">
+        <f>$H$10-C58</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9660,8 +10470,20 @@
       <c r="C59">
         <v>188</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <f>$H$10-C59</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9671,8 +10493,20 @@
       <c r="C60">
         <v>190</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f>$H$10-C60</f>
+        <v>-15.641975308641975</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>244.67139155616519</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9682,8 +10516,20 @@
       <c r="C61">
         <v>191</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <f>$H$10-C61</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9693,8 +10539,20 @@
       <c r="C62">
         <v>191</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <f>$H$10-C62</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9704,8 +10562,20 @@
       <c r="C63">
         <v>191</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <f>$H$10-C63</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9715,8 +10585,20 @@
       <c r="C64">
         <v>193</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <f>$H$10-C64</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9726,8 +10608,20 @@
       <c r="C65">
         <v>193</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <f>$H$10-C65</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -9737,8 +10631,20 @@
       <c r="C66">
         <v>193</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <f>$H$10-C66</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -9748,8 +10654,20 @@
       <c r="C67">
         <v>196</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <f t="shared" ref="D67:D82" si="2">COUNTIF($C$2:$C$82, C67)</f>
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <f>$H$10-C67</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F82" si="3">E67^2</f>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -9759,8 +10677,20 @@
       <c r="C68">
         <v>196</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <f>$H$10-C68</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -9770,8 +10700,20 @@
       <c r="C69">
         <v>196</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <f>$H$10-C69</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -9781,8 +10723,20 @@
       <c r="C70">
         <v>198</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <f>$H$10-C70</f>
+        <v>-23.641975308641975</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>558.94299649443678</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -9792,8 +10746,20 @@
       <c r="C71">
         <v>198</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <f>$H$10-C71</f>
+        <v>-23.641975308641975</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>558.94299649443678</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -9803,8 +10769,20 @@
       <c r="C72">
         <v>200</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <f>$H$10-C72</f>
+        <v>-25.641975308641975</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>657.51089772900468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -9814,8 +10792,20 @@
       <c r="C73">
         <v>202</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <f>$H$10-C73</f>
+        <v>-27.641975308641975</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>764.07879896357258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -9825,8 +10815,20 @@
       <c r="C74">
         <v>206</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <f>$H$10-C74</f>
+        <v>-31.641975308641975</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>1001.2146014327084</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -9836,8 +10838,20 @@
       <c r="C75">
         <v>206</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <f>$H$10-C75</f>
+        <v>-31.641975308641975</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>1001.2146014327084</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -9847,8 +10861,20 @@
       <c r="C76">
         <v>213</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f>$H$10-C76</f>
+        <v>-38.641975308641975</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>1493.2022557536961</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -9858,8 +10884,20 @@
       <c r="C77">
         <v>216</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <f>$H$10-C77</f>
+        <v>-41.641975308641975</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>1734.0541076055479</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -9869,8 +10907,20 @@
       <c r="C78">
         <v>224</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <f>$H$10-C78</f>
+        <v>-49.641975308641975</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>2464.3257125438195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -9880,8 +10930,20 @@
       <c r="C79">
         <v>228</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <f>$H$10-C79</f>
+        <v>-53.641975308641975</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>2877.4615150129553</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -9891,8 +10953,20 @@
       <c r="C80">
         <v>229</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <f>$H$10-C80</f>
+        <v>-54.641975308641975</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>2985.7454656302393</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -9902,8 +10976,20 @@
       <c r="C81">
         <v>234</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <f>$H$10-C81</f>
+        <v>-59.641975308641975</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>3557.1652187166592</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -9912,6 +10998,18 @@
       </c>
       <c r="C82">
         <v>264</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <f>$H$10-C82</f>
+        <v>-89.641975308641975</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>8035.6837372351774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>